<commit_message>
Started the 3d model
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Documents\work-sign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8304C50-A25F-4688-866E-C4C62E367A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B16DF8-631C-48E6-BEBA-D2F53D2824E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{65FF75E3-ED98-4EE0-A10A-1D060FB74263}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -64,9 +77,6 @@
     <t>Switching Power Supply Lighting Transformer</t>
   </si>
   <si>
-    <t>12v Power Supply</t>
-  </si>
-  <si>
     <t>60W/80W Electric Soldering Iron</t>
   </si>
   <si>
@@ -77,6 +87,9 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/1005007087317638.html</t>
+  </si>
+  <si>
+    <t>12v 2A Power Supply</t>
   </si>
 </sst>
 </file>
@@ -952,7 +965,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,32 +1056,32 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>6.58</v>
+        <v>5.22</v>
       </c>
       <c r="E4">
         <f>C4*D4</f>
-        <v>6.58</v>
+        <v>5.22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4">
         <f>ROUND(E4*1.12,2)+G3</f>
-        <v>18.810000000000002</v>
+        <v>17.29</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1081,11 +1094,11 @@
         <v>10.23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5">
         <f>ROUND(E5*1.12,2)+G4</f>
-        <v>30.270000000000003</v>
+        <v>28.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>